<commit_message>
Updated data inputs to fix bugs
</commit_message>
<xml_diff>
--- a/dashboard/Data/Cooking.xlsx
+++ b/dashboard/Data/Cooking.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>OSEMOSYS</t>
   </si>
@@ -72,16 +72,13 @@
     <t>Natural Gas stoves</t>
   </si>
   <si>
-    <t>Solar thermal</t>
-  </si>
-  <si>
-    <t>Solar thermal heating</t>
-  </si>
-  <si>
-    <t>Solar</t>
-  </si>
-  <si>
-    <t>RES_CWH_SOLAR</t>
+    <t>Biomass stoves</t>
+  </si>
+  <si>
+    <t>RES_CWH_BIO_001</t>
+  </si>
+  <si>
+    <t>Biomass</t>
   </si>
 </sst>
 </file>
@@ -456,7 +453,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -545,10 +542,10 @@
         <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
fixed bugs in data download
</commit_message>
<xml_diff>
--- a/dashboard/Data/Cooking.xlsx
+++ b/dashboard/Data/Cooking.xlsx
@@ -24,9 +24,6 @@
     <t>OSEMOSYS</t>
   </si>
   <si>
-    <t>VISUALIZATION</t>
-  </si>
-  <si>
     <t>Use</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>Biomass</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -466,16 +466,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="4"/>
       <c r="H1" s="4"/>
@@ -483,72 +483,72 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected mistake in emission limit in CP and SDG7 scenario, corrected scenario descriptions
</commit_message>
<xml_diff>
--- a/dashboard/Data/Cooking.xlsx
+++ b/dashboard/Data/Cooking.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>OSEMOSYS</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>Solar cookers</t>
+  </si>
+  <si>
+    <t>RES_CWH_SOLAR</t>
+  </si>
+  <si>
+    <t>Solar stoves</t>
+  </si>
+  <si>
+    <t>Solar</t>
   </si>
 </sst>
 </file>
@@ -450,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -551,6 +563,20 @@
         <v>18</v>
       </c>
     </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>